<commit_message>
Updated ITA model - 2025-07-30 09:34
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_andHydro.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_andHydro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9182E131-AA0E-4161-B6BE-0117C3776C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2509BEA-6006-4BC7-95D8-BD54143ACBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="misc" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="234">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -1354,7 +1354,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{034C1C47-C7B1-48B4-9602-2B825216B37E}">
   <dimension ref="B2:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -1849,71 +1851,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5417F31-D792-47CD-82F2-E942FCB1F74A}">
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="11.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.265625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17.25" thickBot="1">
+    <row r="1" spans="1:14" ht="17.25" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="14.65" thickTop="1">
-      <c r="A2" t="s">
+    <row r="2" spans="1:14" ht="14.65" thickTop="1">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" t="s">
         <v>108</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" t="s">
         <v>229</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" t="s">
         <v>230</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1932,26 +1924,26 @@
       <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>111</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>30</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>232</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>0.10575000000000001</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>88.954992178647728</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>0.13359574468085106</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1970,26 +1962,26 @@
       <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>113</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>30</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>232</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>8.9249999999999972</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>88.954992178647728</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>0.14318857142857147</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2008,26 +2000,26 @@
       <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>115</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>30</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>232</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>8.76525</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>0</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>0.15363027295285359</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2046,26 +2038,26 @@
       <c r="F6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>117</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>30</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>232</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>144.17400000000001</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>88.954992178647728</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>0.14922804215739316</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2084,26 +2076,26 @@
       <c r="F7" t="s">
         <v>20</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>119</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>30</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>232</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>83.828999999999994</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>0</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>0.16044121962566654</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2122,26 +2114,26 @@
       <c r="F8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>121</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>30</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>232</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>35.101499999999994</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>88.954992178647728</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>0.1596321524721166</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2160,26 +2152,26 @@
       <c r="F9" t="s">
         <v>20</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>123</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>30</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>232</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>67.489499999999978</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>0</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>0.16821592247682973</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2198,26 +2190,26 @@
       <c r="F10" t="s">
         <v>20</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>125</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>30</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>232</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>1.9597500000000001</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>88.954992178647728</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>0.16538767699961729</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2236,26 +2228,26 @@
       <c r="F11" t="s">
         <v>20</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>127</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>30</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>232</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>8.8425000000000011</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>0</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>0.17716310432569973</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2274,26 +2266,26 @@
       <c r="F12" t="s">
         <v>20</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
         <v>129</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
         <v>31</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
         <v>233</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>13.104750000000001</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>105.74751621237203</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>0.18033772105534251</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2312,26 +2304,26 @@
       <c r="F13" t="s">
         <v>20</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>131</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" t="s">
         <v>31</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>233</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>30.602250000000002</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>145.23264029166972</v>
       </c>
-      <c r="L13">
+      <c r="N13">
         <v>0.1787710217385976</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2350,26 +2342,26 @@
       <c r="F14" t="s">
         <v>20</v>
       </c>
-      <c r="G14" t="s">
+      <c r="I14" t="s">
         <v>133</v>
       </c>
-      <c r="H14" t="s">
+      <c r="J14" t="s">
         <v>31</v>
       </c>
-      <c r="I14" t="s">
+      <c r="K14" t="s">
         <v>233</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <v>1.2044999999999999</v>
       </c>
-      <c r="K14">
+      <c r="M14">
         <v>80.785656162241295</v>
       </c>
-      <c r="L14">
+      <c r="N14">
         <v>0.19397011207970113</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2388,26 +2380,26 @@
       <c r="F15" t="s">
         <v>20</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>135</v>
       </c>
-      <c r="H15" t="s">
+      <c r="J15" t="s">
         <v>31</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>233</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <v>6.1574999999999998</v>
       </c>
-      <c r="K15">
+      <c r="M15">
         <v>105.74751621237203</v>
       </c>
-      <c r="L15">
+      <c r="N15">
         <v>0.18899999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2426,26 +2418,26 @@
       <c r="F16" t="s">
         <v>20</v>
       </c>
-      <c r="G16" t="s">
+      <c r="I16" t="s">
         <v>137</v>
       </c>
-      <c r="H16" t="s">
+      <c r="J16" t="s">
         <v>31</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>233</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <v>26.166</v>
       </c>
-      <c r="K16">
+      <c r="M16">
         <v>145.23264029166972</v>
       </c>
-      <c r="L16">
+      <c r="N16">
         <v>0.19002806122448979</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2464,26 +2456,26 @@
       <c r="F17" t="s">
         <v>20</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
         <v>139</v>
       </c>
-      <c r="H17" t="s">
+      <c r="J17" t="s">
         <v>31</v>
       </c>
-      <c r="I17" t="s">
+      <c r="K17" t="s">
         <v>233</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <v>1.00875</v>
       </c>
-      <c r="K17">
+      <c r="M17">
         <v>80.785656162241295</v>
       </c>
-      <c r="L17">
+      <c r="N17">
         <v>0.19844758364312268</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2502,26 +2494,26 @@
       <c r="F18" t="s">
         <v>20</v>
       </c>
-      <c r="G18" t="s">
+      <c r="I18" t="s">
         <v>141</v>
       </c>
-      <c r="H18" t="s">
+      <c r="J18" t="s">
         <v>31</v>
       </c>
-      <c r="I18" t="s">
+      <c r="K18" t="s">
         <v>233</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <v>27.485249999999997</v>
       </c>
-      <c r="K18">
+      <c r="M18">
         <v>105.74751621237203</v>
       </c>
-      <c r="L18">
+      <c r="N18">
         <v>0.20059120801156985</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2540,26 +2532,26 @@
       <c r="F19" t="s">
         <v>20</v>
       </c>
-      <c r="G19" t="s">
+      <c r="I19" t="s">
         <v>143</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J19" t="s">
         <v>31</v>
       </c>
-      <c r="I19" t="s">
+      <c r="K19" t="s">
         <v>233</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <v>35.112749999999998</v>
       </c>
-      <c r="K19">
+      <c r="M19">
         <v>145.23264029166972</v>
       </c>
-      <c r="L19">
+      <c r="N19">
         <v>0.20057184356109969</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2578,26 +2570,26 @@
       <c r="F20" t="s">
         <v>20</v>
       </c>
-      <c r="G20" t="s">
+      <c r="I20" t="s">
         <v>145</v>
       </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>31</v>
       </c>
-      <c r="I20" t="s">
+      <c r="K20" t="s">
         <v>233</v>
       </c>
-      <c r="J20">
+      <c r="L20">
         <v>12.88425</v>
       </c>
-      <c r="K20">
+      <c r="M20">
         <v>80.785656162241295</v>
       </c>
-      <c r="L20">
+      <c r="N20">
         <v>0.20899999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2616,26 +2608,26 @@
       <c r="F21" t="s">
         <v>20</v>
       </c>
-      <c r="G21" t="s">
+      <c r="I21" t="s">
         <v>147</v>
       </c>
-      <c r="H21" t="s">
+      <c r="J21" t="s">
         <v>31</v>
       </c>
-      <c r="I21" t="s">
+      <c r="K21" t="s">
         <v>233</v>
       </c>
-      <c r="J21">
+      <c r="L21">
         <v>14.06175</v>
       </c>
-      <c r="K21">
+      <c r="M21">
         <v>105.74751621237203</v>
       </c>
-      <c r="L21">
+      <c r="N21">
         <v>0.21141591551549416</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2654,26 +2646,26 @@
       <c r="F22" t="s">
         <v>20</v>
       </c>
-      <c r="G22" t="s">
+      <c r="I22" t="s">
         <v>149</v>
       </c>
-      <c r="H22" t="s">
+      <c r="J22" t="s">
         <v>31</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>233</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <v>16.8705</v>
       </c>
-      <c r="K22">
+      <c r="M22">
         <v>145.23264029166972</v>
       </c>
-      <c r="L22">
+      <c r="N22">
         <v>0.20917453543167067</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2692,26 +2684,26 @@
       <c r="F23" t="s">
         <v>20</v>
       </c>
-      <c r="G23" t="s">
+      <c r="I23" t="s">
         <v>151</v>
       </c>
-      <c r="H23" t="s">
+      <c r="J23" t="s">
         <v>31</v>
       </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
         <v>233</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <v>0.58650000000000002</v>
       </c>
-      <c r="K23">
+      <c r="M23">
         <v>0</v>
       </c>
-      <c r="L23">
+      <c r="N23">
         <v>0.222</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2730,26 +2722,26 @@
       <c r="F24" t="s">
         <v>20</v>
       </c>
-      <c r="G24" t="s">
+      <c r="I24" t="s">
         <v>153</v>
       </c>
-      <c r="H24" t="s">
+      <c r="J24" t="s">
         <v>31</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
         <v>233</v>
       </c>
-      <c r="J24">
+      <c r="L24">
         <v>7.5187499999999998</v>
       </c>
-      <c r="K24">
+      <c r="M24">
         <v>80.785656162241295</v>
       </c>
-      <c r="L24">
+      <c r="N24">
         <v>0.22001067331670823</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -2768,26 +2760,26 @@
       <c r="F25" t="s">
         <v>20</v>
       </c>
-      <c r="G25" t="s">
+      <c r="I25" t="s">
         <v>155</v>
       </c>
-      <c r="H25" t="s">
+      <c r="J25" t="s">
         <v>31</v>
       </c>
-      <c r="I25" t="s">
+      <c r="K25" t="s">
         <v>233</v>
       </c>
-      <c r="J25">
+      <c r="L25">
         <v>20.756250000000001</v>
       </c>
-      <c r="K25">
+      <c r="M25">
         <v>105.74751621237203</v>
       </c>
-      <c r="L25">
+      <c r="N25">
         <v>0.21966670280036132</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -2806,26 +2798,26 @@
       <c r="F26" t="s">
         <v>20</v>
       </c>
-      <c r="G26" t="s">
+      <c r="I26" t="s">
         <v>157</v>
       </c>
-      <c r="H26" t="s">
+      <c r="J26" t="s">
         <v>31</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
         <v>233</v>
       </c>
-      <c r="J26">
+      <c r="L26">
         <v>14.604749999999999</v>
       </c>
-      <c r="K26">
+      <c r="M26">
         <v>145.23264029166972</v>
       </c>
-      <c r="L26">
+      <c r="N26">
         <v>0.21763482771016279</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -2844,26 +2836,26 @@
       <c r="F27" t="s">
         <v>20</v>
       </c>
-      <c r="G27" t="s">
+      <c r="I27" t="s">
         <v>159</v>
       </c>
-      <c r="H27" t="s">
+      <c r="J27" t="s">
         <v>31</v>
       </c>
-      <c r="I27" t="s">
+      <c r="K27" t="s">
         <v>233</v>
       </c>
-      <c r="J27">
+      <c r="L27">
         <v>8.3249999999999993</v>
       </c>
-      <c r="K27">
+      <c r="M27">
         <v>0</v>
       </c>
-      <c r="L27">
+      <c r="N27">
         <v>0.23295243243243247</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -2882,26 +2874,26 @@
       <c r="F28" t="s">
         <v>20</v>
       </c>
-      <c r="G28" t="s">
+      <c r="I28" t="s">
         <v>161</v>
       </c>
-      <c r="H28" t="s">
+      <c r="J28" t="s">
         <v>31</v>
       </c>
-      <c r="I28" t="s">
+      <c r="K28" t="s">
         <v>233</v>
       </c>
-      <c r="J28">
+      <c r="L28">
         <v>10.64025</v>
       </c>
-      <c r="K28">
+      <c r="M28">
         <v>80.785656162241295</v>
       </c>
-      <c r="L28">
+      <c r="N28">
         <v>0.22989025163882429</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -2920,26 +2912,26 @@
       <c r="F29" t="s">
         <v>20</v>
       </c>
-      <c r="G29" t="s">
+      <c r="I29" t="s">
         <v>163</v>
       </c>
-      <c r="H29" t="s">
+      <c r="J29" t="s">
         <v>31</v>
       </c>
-      <c r="I29" t="s">
+      <c r="K29" t="s">
         <v>233</v>
       </c>
-      <c r="J29">
+      <c r="L29">
         <v>21.09675</v>
       </c>
-      <c r="K29">
+      <c r="M29">
         <v>105.74751621237203</v>
       </c>
-      <c r="L29">
+      <c r="N29">
         <v>0.22755778733691209</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -2958,26 +2950,26 @@
       <c r="F30" t="s">
         <v>20</v>
       </c>
-      <c r="G30" t="s">
+      <c r="I30" t="s">
         <v>165</v>
       </c>
-      <c r="H30" t="s">
+      <c r="J30" t="s">
         <v>31</v>
       </c>
-      <c r="I30" t="s">
+      <c r="K30" t="s">
         <v>233</v>
       </c>
-      <c r="J30">
+      <c r="L30">
         <v>13.338000000000001</v>
       </c>
-      <c r="K30">
+      <c r="M30">
         <v>145.23264029166972</v>
       </c>
-      <c r="L30">
+      <c r="N30">
         <v>0.22817026540710753</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -2996,26 +2988,26 @@
       <c r="F31" t="s">
         <v>20</v>
       </c>
-      <c r="G31" t="s">
+      <c r="I31" t="s">
         <v>167</v>
       </c>
-      <c r="H31" t="s">
+      <c r="J31" t="s">
         <v>31</v>
       </c>
-      <c r="I31" t="s">
+      <c r="K31" t="s">
         <v>233</v>
       </c>
-      <c r="J31">
+      <c r="L31">
         <v>1.0394999999999999</v>
       </c>
-      <c r="K31">
+      <c r="M31">
         <v>0</v>
       </c>
-      <c r="L31">
+      <c r="N31">
         <v>0.23800000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -3034,26 +3026,26 @@
       <c r="F32" t="s">
         <v>20</v>
       </c>
-      <c r="G32" t="s">
+      <c r="I32" t="s">
         <v>169</v>
       </c>
-      <c r="H32" t="s">
+      <c r="J32" t="s">
         <v>31</v>
       </c>
-      <c r="I32" t="s">
+      <c r="K32" t="s">
         <v>233</v>
       </c>
-      <c r="J32">
+      <c r="L32">
         <v>1.5675000000000001</v>
       </c>
-      <c r="K32">
+      <c r="M32">
         <v>80.785656162241295</v>
       </c>
-      <c r="L32">
+      <c r="N32">
         <v>0.24259330143540669</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:14">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -3072,26 +3064,26 @@
       <c r="F33" t="s">
         <v>20</v>
       </c>
-      <c r="G33" t="s">
+      <c r="I33" t="s">
         <v>171</v>
       </c>
-      <c r="H33" t="s">
+      <c r="J33" t="s">
         <v>31</v>
       </c>
-      <c r="I33" t="s">
+      <c r="K33" t="s">
         <v>233</v>
       </c>
-      <c r="J33">
+      <c r="L33">
         <v>6.8729999999999993</v>
       </c>
-      <c r="K33">
+      <c r="M33">
         <v>105.74751621237203</v>
       </c>
-      <c r="L33">
+      <c r="N33">
         <v>0.24198919685726758</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:14">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -3110,26 +3102,26 @@
       <c r="F34" t="s">
         <v>20</v>
       </c>
-      <c r="G34" t="s">
+      <c r="I34" t="s">
         <v>173</v>
       </c>
-      <c r="H34" t="s">
+      <c r="J34" t="s">
         <v>31</v>
       </c>
-      <c r="I34" t="s">
+      <c r="K34" t="s">
         <v>233</v>
       </c>
-      <c r="J34">
+      <c r="L34">
         <v>0.68774999999999997</v>
       </c>
-      <c r="K34">
+      <c r="M34">
         <v>145.23264029166972</v>
       </c>
-      <c r="L34">
+      <c r="N34">
         <v>0.24100000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -3148,26 +3140,26 @@
       <c r="F35" t="s">
         <v>20</v>
       </c>
-      <c r="G35" t="s">
+      <c r="I35" t="s">
         <v>175</v>
       </c>
-      <c r="H35" t="s">
+      <c r="J35" t="s">
         <v>31</v>
       </c>
-      <c r="I35" t="s">
+      <c r="K35" t="s">
         <v>233</v>
       </c>
-      <c r="J35">
+      <c r="L35">
         <v>9.7439999999999998</v>
       </c>
-      <c r="K35">
+      <c r="M35">
         <v>0</v>
       </c>
-      <c r="L35">
+      <c r="N35">
         <v>0.2510413331280788</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -3186,26 +3178,26 @@
       <c r="F36" t="s">
         <v>20</v>
       </c>
-      <c r="G36" t="s">
+      <c r="I36" t="s">
         <v>177</v>
       </c>
-      <c r="H36" t="s">
+      <c r="J36" t="s">
         <v>31</v>
       </c>
-      <c r="I36" t="s">
+      <c r="K36" t="s">
         <v>233</v>
       </c>
-      <c r="J36">
+      <c r="L36">
         <v>0.10575</v>
       </c>
-      <c r="K36">
+      <c r="M36">
         <v>0</v>
       </c>
-      <c r="L36">
+      <c r="N36">
         <v>0.26200000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -3224,26 +3216,26 @@
       <c r="F37" t="s">
         <v>20</v>
       </c>
-      <c r="G37" t="s">
+      <c r="I37" t="s">
         <v>179</v>
       </c>
-      <c r="H37" t="s">
+      <c r="J37" t="s">
         <v>31</v>
       </c>
-      <c r="I37" t="s">
+      <c r="K37" t="s">
         <v>233</v>
       </c>
-      <c r="J37">
+      <c r="L37">
         <v>0.12</v>
       </c>
-      <c r="K37">
+      <c r="M37">
         <v>80.785656162241295</v>
       </c>
-      <c r="L37">
+      <c r="N37">
         <v>0.255</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -3262,26 +3254,26 @@
       <c r="F38" t="s">
         <v>20</v>
       </c>
-      <c r="G38" t="s">
+      <c r="I38" t="s">
         <v>181</v>
       </c>
-      <c r="H38" t="s">
+      <c r="J38" t="s">
         <v>31</v>
       </c>
-      <c r="I38" t="s">
+      <c r="K38" t="s">
         <v>233</v>
       </c>
-      <c r="J38">
+      <c r="L38">
         <v>4.725E-2</v>
       </c>
-      <c r="K38">
+      <c r="M38">
         <v>105.74751621237203</v>
       </c>
-      <c r="L38">
+      <c r="N38">
         <v>0.26400000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -3300,26 +3292,26 @@
       <c r="F39" t="s">
         <v>20</v>
       </c>
-      <c r="G39" t="s">
+      <c r="I39" t="s">
         <v>183</v>
       </c>
-      <c r="H39" t="s">
+      <c r="J39" t="s">
         <v>31</v>
       </c>
-      <c r="I39" t="s">
+      <c r="K39" t="s">
         <v>233</v>
       </c>
-      <c r="J39">
+      <c r="L39">
         <v>1.3492500000000001</v>
       </c>
-      <c r="K39">
+      <c r="M39">
         <v>80.785656162241295</v>
       </c>
-      <c r="L39">
+      <c r="N39">
         <v>0.26900000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -3338,26 +3330,26 @@
       <c r="F40" t="s">
         <v>20</v>
       </c>
-      <c r="G40" t="s">
+      <c r="I40" t="s">
         <v>185</v>
       </c>
-      <c r="H40" t="s">
+      <c r="J40" t="s">
         <v>31</v>
       </c>
-      <c r="I40" t="s">
+      <c r="K40" t="s">
         <v>233</v>
       </c>
-      <c r="J40">
+      <c r="L40">
         <v>6.4192499999999999</v>
       </c>
-      <c r="K40">
+      <c r="M40">
         <v>105.74751621237203</v>
       </c>
-      <c r="L40">
+      <c r="N40">
         <v>0.26500000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -3376,26 +3368,26 @@
       <c r="F41" t="s">
         <v>20</v>
       </c>
-      <c r="G41" t="s">
+      <c r="I41" t="s">
         <v>187</v>
       </c>
-      <c r="H41" t="s">
+      <c r="J41" t="s">
         <v>31</v>
       </c>
-      <c r="I41" t="s">
+      <c r="K41" t="s">
         <v>233</v>
       </c>
-      <c r="J41">
+      <c r="L41">
         <v>3.0907499999999999</v>
       </c>
-      <c r="K41">
+      <c r="M41">
         <v>0</v>
       </c>
-      <c r="L41">
+      <c r="N41">
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -3414,26 +3406,26 @@
       <c r="F42" t="s">
         <v>20</v>
       </c>
-      <c r="G42" t="s">
+      <c r="I42" t="s">
         <v>189</v>
       </c>
-      <c r="H42" t="s">
+      <c r="J42" t="s">
         <v>31</v>
       </c>
-      <c r="I42" t="s">
+      <c r="K42" t="s">
         <v>233</v>
       </c>
-      <c r="J42">
+      <c r="L42">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="K42">
+      <c r="M42">
         <v>80.785656162241295</v>
       </c>
-      <c r="L42">
+      <c r="N42">
         <v>0.27800000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -3452,26 +3444,26 @@
       <c r="F43" t="s">
         <v>20</v>
       </c>
-      <c r="G43" t="s">
+      <c r="I43" t="s">
         <v>191</v>
       </c>
-      <c r="H43" t="s">
+      <c r="J43" t="s">
         <v>31</v>
       </c>
-      <c r="I43" t="s">
+      <c r="K43" t="s">
         <v>233</v>
       </c>
-      <c r="J43">
+      <c r="L43">
         <v>0.63900000000000001</v>
       </c>
-      <c r="K43">
+      <c r="M43">
         <v>0</v>
       </c>
-      <c r="L43">
+      <c r="N43">
         <v>0.29273826291079807</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:14">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -3490,26 +3482,26 @@
       <c r="F44" t="s">
         <v>20</v>
       </c>
-      <c r="G44" t="s">
+      <c r="I44" t="s">
         <v>193</v>
       </c>
-      <c r="H44" t="s">
+      <c r="J44" t="s">
         <v>31</v>
       </c>
-      <c r="I44" t="s">
+      <c r="K44" t="s">
         <v>233</v>
       </c>
-      <c r="J44">
+      <c r="L44">
         <v>6.6359999999999992</v>
       </c>
-      <c r="K44">
+      <c r="M44">
         <v>80.785656162241295</v>
       </c>
-      <c r="L44">
+      <c r="N44">
         <v>0.28799999999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:14">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -3528,26 +3520,26 @@
       <c r="F45" t="s">
         <v>20</v>
       </c>
-      <c r="G45" t="s">
+      <c r="I45" t="s">
         <v>195</v>
       </c>
-      <c r="H45" t="s">
+      <c r="J45" t="s">
         <v>31</v>
       </c>
-      <c r="I45" t="s">
+      <c r="K45" t="s">
         <v>233</v>
       </c>
-      <c r="J45">
+      <c r="L45">
         <v>3.9892499999999997</v>
       </c>
-      <c r="K45">
+      <c r="M45">
         <v>0</v>
       </c>
-      <c r="L45">
+      <c r="N45">
         <v>0.30293043805226549</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:14">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -3566,26 +3558,26 @@
       <c r="F46" t="s">
         <v>20</v>
       </c>
-      <c r="G46" t="s">
+      <c r="I46" t="s">
         <v>197</v>
       </c>
-      <c r="H46" t="s">
+      <c r="J46" t="s">
         <v>31</v>
       </c>
-      <c r="I46" t="s">
+      <c r="K46" t="s">
         <v>233</v>
       </c>
-      <c r="J46">
+      <c r="L46">
         <v>2.5357500000000002</v>
       </c>
-      <c r="K46">
+      <c r="M46">
         <v>0</v>
       </c>
-      <c r="L46">
+      <c r="N46">
         <v>0.32197219757468204</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:14">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -3604,26 +3596,26 @@
       <c r="F47" t="s">
         <v>20</v>
       </c>
-      <c r="G47" t="s">
+      <c r="I47" t="s">
         <v>199</v>
       </c>
-      <c r="H47" t="s">
+      <c r="J47" t="s">
         <v>31</v>
       </c>
-      <c r="I47" t="s">
+      <c r="K47" t="s">
         <v>233</v>
       </c>
-      <c r="J47">
+      <c r="L47">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="K47">
+      <c r="M47">
         <v>0</v>
       </c>
-      <c r="L47">
+      <c r="N47">
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -3642,26 +3634,26 @@
       <c r="F48" t="s">
         <v>20</v>
       </c>
-      <c r="G48" t="s">
+      <c r="I48" t="s">
         <v>201</v>
       </c>
-      <c r="H48" t="s">
+      <c r="J48" t="s">
         <v>31</v>
       </c>
-      <c r="I48" t="s">
+      <c r="K48" t="s">
         <v>233</v>
       </c>
-      <c r="J48">
+      <c r="L48">
         <v>1.2E-2</v>
       </c>
-      <c r="K48">
+      <c r="M48">
         <v>105.74751621237203</v>
       </c>
-      <c r="L48">
+      <c r="N48">
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -3680,26 +3672,26 @@
       <c r="F49" t="s">
         <v>20</v>
       </c>
-      <c r="G49" t="s">
+      <c r="I49" t="s">
         <v>203</v>
       </c>
-      <c r="H49" t="s">
+      <c r="J49" t="s">
         <v>31</v>
       </c>
-      <c r="I49" t="s">
+      <c r="K49" t="s">
         <v>233</v>
       </c>
-      <c r="J49">
+      <c r="L49">
         <v>7.4249999999999997E-2</v>
       </c>
-      <c r="K49">
+      <c r="M49">
         <v>0</v>
       </c>
-      <c r="L49">
+      <c r="N49">
         <v>0.35</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
         <v>19</v>
       </c>
@@ -3718,26 +3710,26 @@
       <c r="F50" t="s">
         <v>20</v>
       </c>
-      <c r="G50" t="s">
+      <c r="I50" t="s">
         <v>205</v>
       </c>
-      <c r="H50" t="s">
+      <c r="J50" t="s">
         <v>31</v>
       </c>
-      <c r="I50" t="s">
+      <c r="K50" t="s">
         <v>233</v>
       </c>
-      <c r="J50">
+      <c r="L50">
         <v>10.199249999999999</v>
       </c>
-      <c r="K50">
+      <c r="M50">
         <v>199.69488040104588</v>
       </c>
-      <c r="L50">
+      <c r="N50">
         <v>0.3014461357452754</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>19</v>
       </c>
@@ -3756,26 +3748,26 @@
       <c r="F51" t="s">
         <v>20</v>
       </c>
-      <c r="G51" t="s">
+      <c r="I51" t="s">
         <v>207</v>
       </c>
-      <c r="H51" t="s">
+      <c r="J51" t="s">
         <v>31</v>
       </c>
-      <c r="I51" t="s">
+      <c r="K51" t="s">
         <v>233</v>
       </c>
-      <c r="J51">
+      <c r="L51">
         <v>28.78725</v>
       </c>
-      <c r="K51">
+      <c r="M51">
         <v>199.69488040104588</v>
       </c>
-      <c r="L51">
+      <c r="N51">
         <v>0.30935359403902762</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -3794,26 +3786,26 @@
       <c r="F52" t="s">
         <v>20</v>
       </c>
-      <c r="G52" t="s">
+      <c r="I52" t="s">
         <v>209</v>
       </c>
-      <c r="H52" t="s">
+      <c r="J52" t="s">
         <v>31</v>
       </c>
-      <c r="I52" t="s">
+      <c r="K52" t="s">
         <v>233</v>
       </c>
-      <c r="J52">
+      <c r="L52">
         <v>46.53</v>
       </c>
-      <c r="K52">
+      <c r="M52">
         <v>199.69488040104588</v>
       </c>
-      <c r="L52">
+      <c r="N52">
         <v>0.32123186653771763</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
         <v>19</v>
       </c>
@@ -3832,26 +3824,26 @@
       <c r="F53" t="s">
         <v>20</v>
       </c>
-      <c r="G53" t="s">
+      <c r="I53" t="s">
         <v>211</v>
       </c>
-      <c r="H53" t="s">
+      <c r="J53" t="s">
         <v>31</v>
       </c>
-      <c r="I53" t="s">
+      <c r="K53" t="s">
         <v>233</v>
       </c>
-      <c r="J53">
+      <c r="L53">
         <v>42.752249999999997</v>
       </c>
-      <c r="K53">
+      <c r="M53">
         <v>199.69488040104588</v>
       </c>
-      <c r="L53">
+      <c r="N53">
         <v>0.32912120414715024</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -3870,26 +3862,26 @@
       <c r="F54" t="s">
         <v>20</v>
       </c>
-      <c r="G54" t="s">
+      <c r="I54" t="s">
         <v>213</v>
       </c>
-      <c r="H54" t="s">
+      <c r="J54" t="s">
         <v>31</v>
       </c>
-      <c r="I54" t="s">
+      <c r="K54" t="s">
         <v>233</v>
       </c>
-      <c r="J54">
+      <c r="L54">
         <v>38.504250000000006</v>
       </c>
-      <c r="K54">
+      <c r="M54">
         <v>199.69488040104588</v>
       </c>
-      <c r="L54">
+      <c r="N54">
         <v>0.3393461306219443</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -3908,26 +3900,26 @@
       <c r="F55" t="s">
         <v>20</v>
       </c>
-      <c r="G55" t="s">
+      <c r="I55" t="s">
         <v>215</v>
       </c>
-      <c r="H55" t="s">
+      <c r="J55" t="s">
         <v>31</v>
       </c>
-      <c r="I55" t="s">
+      <c r="K55" t="s">
         <v>233</v>
       </c>
-      <c r="J55">
+      <c r="L55">
         <v>39.440249999999992</v>
       </c>
-      <c r="K55">
+      <c r="M55">
         <v>199.69488040104588</v>
       </c>
-      <c r="L55">
+      <c r="N55">
         <v>0.35020324414779325</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:14">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -3946,26 +3938,26 @@
       <c r="F56" t="s">
         <v>20</v>
       </c>
-      <c r="G56" t="s">
+      <c r="I56" t="s">
         <v>217</v>
       </c>
-      <c r="H56" t="s">
+      <c r="J56" t="s">
         <v>31</v>
       </c>
-      <c r="I56" t="s">
+      <c r="K56" t="s">
         <v>233</v>
       </c>
-      <c r="J56">
+      <c r="L56">
         <v>22.087500000000006</v>
       </c>
-      <c r="K56">
+      <c r="M56">
         <v>199.69488040104588</v>
       </c>
-      <c r="L56">
+      <c r="N56">
         <v>0.35674427843803047</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -3984,26 +3976,26 @@
       <c r="F57" t="s">
         <v>20</v>
       </c>
-      <c r="G57" t="s">
+      <c r="I57" t="s">
         <v>219</v>
       </c>
-      <c r="H57" t="s">
+      <c r="J57" t="s">
         <v>31</v>
       </c>
-      <c r="I57" t="s">
+      <c r="K57" t="s">
         <v>233</v>
       </c>
-      <c r="J57">
+      <c r="L57">
         <v>13.481249999999999</v>
       </c>
-      <c r="K57">
+      <c r="M57">
         <v>199.69488040104588</v>
       </c>
-      <c r="L57">
+      <c r="N57">
         <v>0.36756244784422809</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -4022,26 +4014,26 @@
       <c r="F58" t="s">
         <v>20</v>
       </c>
-      <c r="G58" t="s">
+      <c r="I58" t="s">
         <v>221</v>
       </c>
-      <c r="H58" t="s">
+      <c r="J58" t="s">
         <v>31</v>
       </c>
-      <c r="I58" t="s">
+      <c r="K58" t="s">
         <v>233</v>
       </c>
-      <c r="J58">
+      <c r="L58">
         <v>6.2872500000000002</v>
       </c>
-      <c r="K58">
+      <c r="M58">
         <v>199.69488040104588</v>
       </c>
-      <c r="L58">
+      <c r="N58">
         <v>0.38500000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:14">
       <c r="A59" t="s">
         <v>19</v>
       </c>
@@ -4060,20 +4052,20 @@
       <c r="F59" t="s">
         <v>16</v>
       </c>
-      <c r="G59" t="s">
+      <c r="I59" t="s">
         <v>223</v>
       </c>
-      <c r="H59" t="s">
+      <c r="J59" t="s">
         <v>32</v>
       </c>
-      <c r="I59" t="s">
+      <c r="K59" t="s">
         <v>21</v>
       </c>
-      <c r="J59">
+      <c r="L59">
         <v>6.1390000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:14">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -4092,20 +4084,20 @@
       <c r="F60" t="s">
         <v>16</v>
       </c>
-      <c r="G60" t="s">
+      <c r="I60" t="s">
         <v>225</v>
       </c>
-      <c r="H60" t="s">
+      <c r="J60" t="s">
         <v>32</v>
       </c>
-      <c r="I60" t="s">
+      <c r="K60" t="s">
         <v>21</v>
       </c>
-      <c r="J60">
+      <c r="L60">
         <v>1.3440000000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:14">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -4124,16 +4116,16 @@
       <c r="F61" t="s">
         <v>16</v>
       </c>
-      <c r="G61" t="s">
+      <c r="I61" t="s">
         <v>227</v>
       </c>
-      <c r="H61" t="s">
+      <c r="J61" t="s">
         <v>32</v>
       </c>
-      <c r="I61" t="s">
+      <c r="K61" t="s">
         <v>21</v>
       </c>
-      <c r="J61">
+      <c r="L61">
         <v>1.131</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-30 13:27
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_andHydro.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_andHydro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BB0832-09C6-4FB5-A325-37649B109371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8F257D-B00A-415F-8947-4D9FB7A55974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="misc" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="235">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>TAct</t>
-  </si>
-  <si>
-    <t>PJ</t>
   </si>
   <si>
     <t>GW</t>
@@ -428,6 +425,9 @@
     <t>~FI_T: USD10~FX~ACT_BND</t>
   </si>
   <si>
+    <t>invcost</t>
+  </si>
+  <si>
     <t>process</t>
   </si>
   <si>
@@ -777,6 +777,9 @@
   </si>
   <si>
     <t>New Hydro Potential - Italy - Step 1</t>
+  </si>
+  <si>
+    <t>PJ</t>
   </si>
   <si>
     <t>EN_Hydro_ITA-2</t>
@@ -1380,7 +1383,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -1404,10 +1407,10 @@
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>2</v>
@@ -1422,7 +1425,7 @@
         <v>5</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P3" s="1">
         <v>2022</v>
@@ -1433,26 +1436,26 @@
     </row>
     <row r="4" spans="2:20">
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
       </c>
       <c r="J4" s="1" t="str">
         <f>C4</f>
         <v>ElcAgg_Solar</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M4" s="1">
         <v>1</v>
@@ -1466,19 +1469,19 @@
     </row>
     <row r="5" spans="2:20">
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1487,7 +1490,7 @@
         <v>ElcAgg_Wind</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M5" s="1">
         <v>1</v>
@@ -1501,17 +1504,17 @@
     </row>
     <row r="6" spans="2:20">
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1521,10 +1524,10 @@
         <v>elc_demand</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M6" s="1">
         <v>1</v>
@@ -1536,22 +1539,22 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="T6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="2:20">
       <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1562,7 +1565,7 @@
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -1577,24 +1580,24 @@
     </row>
     <row r="8" spans="2:20">
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1609,24 +1612,24 @@
     </row>
     <row r="9" spans="2:20">
       <c r="B9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1651,7 +1654,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1676,7 +1679,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -1701,7 +1704,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -1726,7 +1729,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -1751,7 +1754,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1776,7 +1779,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1801,7 +1804,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1820,7 +1823,7 @@
         <v>Trd_electricity import</v>
       </c>
       <c r="L17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -1835,7 +1838,7 @@
         <v>Trd_electricity export</v>
       </c>
       <c r="K18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P18">
         <v>0</v>
@@ -1853,7 +1856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5417F31-D792-47CD-82F2-E942FCB1F74A}">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -1864,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="14.65" thickTop="1">
@@ -1896,18 +1899,18 @@
         <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="M2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="N2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>111</v>
@@ -1916,22 +1919,22 @@
         <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
         <v>111</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L3">
         <v>0.10575000000000001</v>
@@ -1945,7 +1948,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>113</v>
@@ -1954,22 +1957,22 @@
         <v>114</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
         <v>113</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K4" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L4">
         <v>8.9249999999999972</v>
@@ -1983,7 +1986,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>115</v>
@@ -1992,22 +1995,22 @@
         <v>116</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
         <v>115</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L5">
         <v>8.76525</v>
@@ -2021,7 +2024,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>117</v>
@@ -2030,22 +2033,22 @@
         <v>118</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
         <v>117</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L6">
         <v>144.17400000000001</v>
@@ -2059,7 +2062,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>119</v>
@@ -2068,22 +2071,22 @@
         <v>120</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I7" t="s">
         <v>119</v>
       </c>
       <c r="J7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L7">
         <v>83.828999999999994</v>
@@ -2097,7 +2100,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>121</v>
@@ -2106,22 +2109,22 @@
         <v>122</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
         <v>121</v>
       </c>
       <c r="J8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L8">
         <v>35.101499999999994</v>
@@ -2135,7 +2138,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>123</v>
@@ -2144,22 +2147,22 @@
         <v>124</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I9" t="s">
         <v>123</v>
       </c>
       <c r="J9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K9" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L9">
         <v>67.489499999999978</v>
@@ -2173,7 +2176,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>125</v>
@@ -2182,22 +2185,22 @@
         <v>126</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I10" t="s">
         <v>125</v>
       </c>
       <c r="J10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L10">
         <v>1.9597500000000001</v>
@@ -2211,7 +2214,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>127</v>
@@ -2220,22 +2223,22 @@
         <v>128</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I11" t="s">
         <v>127</v>
       </c>
       <c r="J11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K11" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L11">
         <v>8.8425000000000011</v>
@@ -2249,7 +2252,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>129</v>
@@ -2258,22 +2261,22 @@
         <v>130</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I12" t="s">
         <v>129</v>
       </c>
       <c r="J12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L12">
         <v>13.104750000000001</v>
@@ -2287,7 +2290,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>131</v>
@@ -2296,22 +2299,22 @@
         <v>132</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I13" t="s">
         <v>131</v>
       </c>
       <c r="J13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K13" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L13">
         <v>30.602250000000002</v>
@@ -2325,7 +2328,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>133</v>
@@ -2334,22 +2337,22 @@
         <v>134</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I14" t="s">
         <v>133</v>
       </c>
       <c r="J14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K14" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L14">
         <v>1.2044999999999999</v>
@@ -2363,7 +2366,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>135</v>
@@ -2372,22 +2375,22 @@
         <v>136</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I15" t="s">
         <v>135</v>
       </c>
       <c r="J15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K15" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L15">
         <v>6.1574999999999998</v>
@@ -2401,7 +2404,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>137</v>
@@ -2410,22 +2413,22 @@
         <v>138</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I16" t="s">
         <v>137</v>
       </c>
       <c r="J16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K16" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L16">
         <v>26.166</v>
@@ -2439,7 +2442,7 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>139</v>
@@ -2448,22 +2451,22 @@
         <v>140</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I17" t="s">
         <v>139</v>
       </c>
       <c r="J17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K17" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L17">
         <v>1.00875</v>
@@ -2477,7 +2480,7 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>141</v>
@@ -2486,22 +2489,22 @@
         <v>142</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I18" t="s">
         <v>141</v>
       </c>
       <c r="J18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K18" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L18">
         <v>27.485249999999997</v>
@@ -2515,7 +2518,7 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>143</v>
@@ -2524,22 +2527,22 @@
         <v>144</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I19" t="s">
         <v>143</v>
       </c>
       <c r="J19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K19" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L19">
         <v>35.112749999999998</v>
@@ -2553,7 +2556,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>145</v>
@@ -2562,22 +2565,22 @@
         <v>146</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I20" t="s">
         <v>145</v>
       </c>
       <c r="J20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K20" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L20">
         <v>12.88425</v>
@@ -2591,7 +2594,7 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>147</v>
@@ -2600,22 +2603,22 @@
         <v>148</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I21" t="s">
         <v>147</v>
       </c>
       <c r="J21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K21" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L21">
         <v>14.06175</v>
@@ -2629,7 +2632,7 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
         <v>149</v>
@@ -2638,22 +2641,22 @@
         <v>150</v>
       </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I22" t="s">
         <v>149</v>
       </c>
       <c r="J22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K22" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L22">
         <v>16.8705</v>
@@ -2667,7 +2670,7 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>151</v>
@@ -2676,22 +2679,22 @@
         <v>152</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I23" t="s">
         <v>151</v>
       </c>
       <c r="J23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K23" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L23">
         <v>0.58650000000000002</v>
@@ -2705,7 +2708,7 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
         <v>153</v>
@@ -2714,22 +2717,22 @@
         <v>154</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I24" t="s">
         <v>153</v>
       </c>
       <c r="J24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K24" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L24">
         <v>7.5187499999999998</v>
@@ -2743,7 +2746,7 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
         <v>155</v>
@@ -2752,22 +2755,22 @@
         <v>156</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I25" t="s">
         <v>155</v>
       </c>
       <c r="J25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K25" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L25">
         <v>20.756250000000001</v>
@@ -2781,7 +2784,7 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
         <v>157</v>
@@ -2790,22 +2793,22 @@
         <v>158</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I26" t="s">
         <v>157</v>
       </c>
       <c r="J26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K26" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L26">
         <v>14.604749999999999</v>
@@ -2819,7 +2822,7 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
         <v>159</v>
@@ -2828,22 +2831,22 @@
         <v>160</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I27" t="s">
         <v>159</v>
       </c>
       <c r="J27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K27" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L27">
         <v>8.3249999999999993</v>
@@ -2857,7 +2860,7 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
         <v>161</v>
@@ -2866,22 +2869,22 @@
         <v>162</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I28" t="s">
         <v>161</v>
       </c>
       <c r="J28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K28" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L28">
         <v>10.64025</v>
@@ -2895,7 +2898,7 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
         <v>163</v>
@@ -2904,22 +2907,22 @@
         <v>164</v>
       </c>
       <c r="D29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I29" t="s">
         <v>163</v>
       </c>
       <c r="J29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K29" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L29">
         <v>21.09675</v>
@@ -2933,7 +2936,7 @@
     </row>
     <row r="30" spans="1:14">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
         <v>165</v>
@@ -2942,22 +2945,22 @@
         <v>166</v>
       </c>
       <c r="D30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I30" t="s">
         <v>165</v>
       </c>
       <c r="J30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K30" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L30">
         <v>13.338000000000001</v>
@@ -2971,7 +2974,7 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
         <v>167</v>
@@ -2980,22 +2983,22 @@
         <v>168</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I31" t="s">
         <v>167</v>
       </c>
       <c r="J31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K31" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L31">
         <v>1.0394999999999999</v>
@@ -3009,7 +3012,7 @@
     </row>
     <row r="32" spans="1:14">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
         <v>169</v>
@@ -3018,22 +3021,22 @@
         <v>170</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I32" t="s">
         <v>169</v>
       </c>
       <c r="J32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K32" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L32">
         <v>1.5675000000000001</v>
@@ -3047,7 +3050,7 @@
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
         <v>171</v>
@@ -3056,22 +3059,22 @@
         <v>172</v>
       </c>
       <c r="D33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I33" t="s">
         <v>171</v>
       </c>
       <c r="J33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K33" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L33">
         <v>6.8729999999999993</v>
@@ -3085,7 +3088,7 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
         <v>173</v>
@@ -3094,22 +3097,22 @@
         <v>174</v>
       </c>
       <c r="D34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I34" t="s">
         <v>173</v>
       </c>
       <c r="J34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K34" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L34">
         <v>0.68774999999999997</v>
@@ -3123,7 +3126,7 @@
     </row>
     <row r="35" spans="1:14">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
         <v>175</v>
@@ -3132,22 +3135,22 @@
         <v>176</v>
       </c>
       <c r="D35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I35" t="s">
         <v>175</v>
       </c>
       <c r="J35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K35" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L35">
         <v>9.7439999999999998</v>
@@ -3161,7 +3164,7 @@
     </row>
     <row r="36" spans="1:14">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
         <v>177</v>
@@ -3170,22 +3173,22 @@
         <v>178</v>
       </c>
       <c r="D36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I36" t="s">
         <v>177</v>
       </c>
       <c r="J36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K36" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L36">
         <v>0.10575</v>
@@ -3199,7 +3202,7 @@
     </row>
     <row r="37" spans="1:14">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
         <v>179</v>
@@ -3208,22 +3211,22 @@
         <v>180</v>
       </c>
       <c r="D37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I37" t="s">
         <v>179</v>
       </c>
       <c r="J37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K37" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L37">
         <v>0.12</v>
@@ -3237,7 +3240,7 @@
     </row>
     <row r="38" spans="1:14">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
         <v>181</v>
@@ -3246,22 +3249,22 @@
         <v>182</v>
       </c>
       <c r="D38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I38" t="s">
         <v>181</v>
       </c>
       <c r="J38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K38" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L38">
         <v>4.725E-2</v>
@@ -3275,7 +3278,7 @@
     </row>
     <row r="39" spans="1:14">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39" t="s">
         <v>183</v>
@@ -3284,22 +3287,22 @@
         <v>184</v>
       </c>
       <c r="D39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I39" t="s">
         <v>183</v>
       </c>
       <c r="J39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K39" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L39">
         <v>1.3492500000000001</v>
@@ -3313,7 +3316,7 @@
     </row>
     <row r="40" spans="1:14">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
         <v>185</v>
@@ -3322,22 +3325,22 @@
         <v>186</v>
       </c>
       <c r="D40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I40" t="s">
         <v>185</v>
       </c>
       <c r="J40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K40" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L40">
         <v>6.4192499999999999</v>
@@ -3351,7 +3354,7 @@
     </row>
     <row r="41" spans="1:14">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
         <v>187</v>
@@ -3360,22 +3363,22 @@
         <v>188</v>
       </c>
       <c r="D41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I41" t="s">
         <v>187</v>
       </c>
       <c r="J41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K41" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L41">
         <v>3.0907499999999999</v>
@@ -3389,7 +3392,7 @@
     </row>
     <row r="42" spans="1:14">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B42" t="s">
         <v>189</v>
@@ -3398,22 +3401,22 @@
         <v>190</v>
       </c>
       <c r="D42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I42" t="s">
         <v>189</v>
       </c>
       <c r="J42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K42" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L42">
         <v>6.0000000000000001E-3</v>
@@ -3427,7 +3430,7 @@
     </row>
     <row r="43" spans="1:14">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B43" t="s">
         <v>191</v>
@@ -3436,22 +3439,22 @@
         <v>192</v>
       </c>
       <c r="D43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I43" t="s">
         <v>191</v>
       </c>
       <c r="J43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K43" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L43">
         <v>0.63900000000000001</v>
@@ -3465,7 +3468,7 @@
     </row>
     <row r="44" spans="1:14">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B44" t="s">
         <v>193</v>
@@ -3474,22 +3477,22 @@
         <v>194</v>
       </c>
       <c r="D44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I44" t="s">
         <v>193</v>
       </c>
       <c r="J44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K44" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L44">
         <v>6.6359999999999992</v>
@@ -3503,7 +3506,7 @@
     </row>
     <row r="45" spans="1:14">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B45" t="s">
         <v>195</v>
@@ -3512,22 +3515,22 @@
         <v>196</v>
       </c>
       <c r="D45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I45" t="s">
         <v>195</v>
       </c>
       <c r="J45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K45" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L45">
         <v>3.9892499999999997</v>
@@ -3541,7 +3544,7 @@
     </row>
     <row r="46" spans="1:14">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B46" t="s">
         <v>197</v>
@@ -3550,22 +3553,22 @@
         <v>198</v>
       </c>
       <c r="D46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I46" t="s">
         <v>197</v>
       </c>
       <c r="J46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K46" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L46">
         <v>2.5357500000000002</v>
@@ -3579,7 +3582,7 @@
     </row>
     <row r="47" spans="1:14">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
         <v>199</v>
@@ -3588,22 +3591,22 @@
         <v>200</v>
       </c>
       <c r="D47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I47" t="s">
         <v>199</v>
       </c>
       <c r="J47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K47" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L47">
         <v>1.7999999999999999E-2</v>
@@ -3617,7 +3620,7 @@
     </row>
     <row r="48" spans="1:14">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B48" t="s">
         <v>201</v>
@@ -3626,22 +3629,22 @@
         <v>202</v>
       </c>
       <c r="D48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I48" t="s">
         <v>201</v>
       </c>
       <c r="J48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K48" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L48">
         <v>1.2E-2</v>
@@ -3655,7 +3658,7 @@
     </row>
     <row r="49" spans="1:14">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49" t="s">
         <v>203</v>
@@ -3664,22 +3667,22 @@
         <v>204</v>
       </c>
       <c r="D49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I49" t="s">
         <v>203</v>
       </c>
       <c r="J49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K49" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L49">
         <v>7.4249999999999997E-2</v>
@@ -3693,7 +3696,7 @@
     </row>
     <row r="50" spans="1:14">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B50" t="s">
         <v>205</v>
@@ -3702,22 +3705,22 @@
         <v>206</v>
       </c>
       <c r="D50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I50" t="s">
         <v>205</v>
       </c>
       <c r="J50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K50" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L50">
         <v>10.199249999999999</v>
@@ -3731,7 +3734,7 @@
     </row>
     <row r="51" spans="1:14">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B51" t="s">
         <v>207</v>
@@ -3740,22 +3743,22 @@
         <v>208</v>
       </c>
       <c r="D51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I51" t="s">
         <v>207</v>
       </c>
       <c r="J51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K51" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L51">
         <v>28.78725</v>
@@ -3769,7 +3772,7 @@
     </row>
     <row r="52" spans="1:14">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B52" t="s">
         <v>209</v>
@@ -3778,22 +3781,22 @@
         <v>210</v>
       </c>
       <c r="D52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I52" t="s">
         <v>209</v>
       </c>
       <c r="J52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K52" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L52">
         <v>46.53</v>
@@ -3807,7 +3810,7 @@
     </row>
     <row r="53" spans="1:14">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B53" t="s">
         <v>211</v>
@@ -3816,22 +3819,22 @@
         <v>212</v>
       </c>
       <c r="D53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I53" t="s">
         <v>211</v>
       </c>
       <c r="J53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K53" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L53">
         <v>42.752249999999997</v>
@@ -3845,7 +3848,7 @@
     </row>
     <row r="54" spans="1:14">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B54" t="s">
         <v>213</v>
@@ -3854,22 +3857,22 @@
         <v>214</v>
       </c>
       <c r="D54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E54" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I54" t="s">
         <v>213</v>
       </c>
       <c r="J54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K54" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L54">
         <v>38.504250000000006</v>
@@ -3883,7 +3886,7 @@
     </row>
     <row r="55" spans="1:14">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B55" t="s">
         <v>215</v>
@@ -3892,22 +3895,22 @@
         <v>216</v>
       </c>
       <c r="D55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I55" t="s">
         <v>215</v>
       </c>
       <c r="J55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K55" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L55">
         <v>39.440249999999992</v>
@@ -3921,7 +3924,7 @@
     </row>
     <row r="56" spans="1:14">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B56" t="s">
         <v>217</v>
@@ -3930,22 +3933,22 @@
         <v>218</v>
       </c>
       <c r="D56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I56" t="s">
         <v>217</v>
       </c>
       <c r="J56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K56" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L56">
         <v>22.087500000000006</v>
@@ -3959,7 +3962,7 @@
     </row>
     <row r="57" spans="1:14">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B57" t="s">
         <v>219</v>
@@ -3968,22 +3971,22 @@
         <v>220</v>
       </c>
       <c r="D57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F57" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I57" t="s">
         <v>219</v>
       </c>
       <c r="J57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K57" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L57">
         <v>13.481249999999999</v>
@@ -3997,7 +4000,7 @@
     </row>
     <row r="58" spans="1:14">
       <c r="A58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B58" t="s">
         <v>221</v>
@@ -4006,22 +4009,22 @@
         <v>222</v>
       </c>
       <c r="D58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F58" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I58" t="s">
         <v>221</v>
       </c>
       <c r="J58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K58" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L58">
         <v>6.2872500000000002</v>
@@ -4035,7 +4038,7 @@
     </row>
     <row r="59" spans="1:14">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B59" t="s">
         <v>223</v>
@@ -4044,22 +4047,22 @@
         <v>224</v>
       </c>
       <c r="D59" t="s">
-        <v>10</v>
+        <v>225</v>
       </c>
       <c r="E59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I59" t="s">
         <v>223</v>
       </c>
       <c r="J59" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K59" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L59">
         <v>6.1390000000000002</v>
@@ -4067,31 +4070,31 @@
     </row>
     <row r="60" spans="1:14">
       <c r="A60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B60" t="s">
+        <v>226</v>
+      </c>
+      <c r="C60" t="s">
+        <v>227</v>
+      </c>
+      <c r="D60" t="s">
         <v>225</v>
       </c>
-      <c r="C60" t="s">
+      <c r="E60" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" t="s">
+        <v>15</v>
+      </c>
+      <c r="I60" t="s">
         <v>226</v>
       </c>
-      <c r="D60" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" t="s">
-        <v>11</v>
-      </c>
-      <c r="F60" t="s">
-        <v>16</v>
-      </c>
-      <c r="I60" t="s">
-        <v>225</v>
-      </c>
       <c r="J60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L60">
         <v>1.3440000000000001</v>
@@ -4099,31 +4102,31 @@
     </row>
     <row r="61" spans="1:14">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B61" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C61" t="s">
+        <v>229</v>
+      </c>
+      <c r="D61" t="s">
+        <v>225</v>
+      </c>
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" t="s">
+        <v>15</v>
+      </c>
+      <c r="I61" t="s">
         <v>228</v>
       </c>
-      <c r="D61" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" t="s">
-        <v>11</v>
-      </c>
-      <c r="F61" t="s">
-        <v>16</v>
-      </c>
-      <c r="I61" t="s">
-        <v>227</v>
-      </c>
       <c r="J61" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L61">
         <v>1.131</v>
@@ -4166,7 +4169,7 @@
   <sheetData>
     <row r="2" spans="2:23">
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -4178,63 +4181,63 @@
     </row>
     <row r="3" spans="2:23">
       <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="2:23">
       <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="2:23">
       <c r="C5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:23">
@@ -4252,7 +4255,7 @@
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
@@ -4275,29 +4278,29 @@
         <v>7</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="G9" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7" t="s">
         <v>1</v>
       </c>
       <c r="J9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="L9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="N9" s="7">
         <f>J35</f>
@@ -4331,46 +4334,46 @@
         <v>3</v>
       </c>
       <c r="V9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="W9" t="s">
         <v>62</v>
-      </c>
-      <c r="W9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="2:23">
       <c r="B10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>66</v>
-      </c>
       <c r="E10" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="K10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N10" s="10">
         <f>1/N17</f>
@@ -4394,35 +4397,35 @@
     <row r="11" spans="2:23">
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="K11" s="7" t="s">
-        <v>71</v>
-      </c>
       <c r="L11" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N11" s="10">
         <f>4/24</f>
@@ -4448,17 +4451,17 @@
       <c r="G12" s="6"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N12" s="10">
         <v>1</v>
@@ -4481,10 +4484,10 @@
       <c r="G13" s="6"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
@@ -4522,10 +4525,10 @@
     </row>
     <row r="14" spans="2:23">
       <c r="I14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N14" s="4">
         <f>J44</f>
@@ -4558,13 +4561,13 @@
     </row>
     <row r="15" spans="2:23">
       <c r="I15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N15" s="4">
         <v>1</v>
@@ -4578,10 +4581,10 @@
     </row>
     <row r="16" spans="2:23">
       <c r="I16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N16" s="10">
         <v>31.536000000000001</v>
@@ -4595,10 +4598,10 @@
     </row>
     <row r="17" spans="9:23">
       <c r="I17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N17" s="4">
         <v>0.85</v>
@@ -4612,19 +4615,19 @@
     </row>
     <row r="18" spans="9:23">
       <c r="I18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N18" s="10">
         <f>1/N25</f>
@@ -4647,19 +4650,19 @@
     </row>
     <row r="19" spans="9:23">
       <c r="I19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J19" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19" t="s">
         <v>70</v>
       </c>
-      <c r="K19" t="s">
-        <v>71</v>
-      </c>
       <c r="L19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N19" s="4">
         <f>8/24</f>
@@ -4678,16 +4681,16 @@
     </row>
     <row r="20" spans="9:23">
       <c r="I20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N20" s="4">
         <v>1</v>
@@ -4701,10 +4704,10 @@
     </row>
     <row r="21" spans="9:23">
       <c r="I21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N21" s="4">
         <f>J49</f>
@@ -4737,10 +4740,10 @@
     </row>
     <row r="22" spans="9:23">
       <c r="I22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N22" s="4">
         <f>J53</f>
@@ -4773,13 +4776,13 @@
     </row>
     <row r="23" spans="9:23">
       <c r="I23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N23" s="4">
         <v>1</v>
@@ -4793,10 +4796,10 @@
     </row>
     <row r="24" spans="9:23">
       <c r="I24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N24" s="10">
         <v>31.536000000000001</v>
@@ -4810,10 +4813,10 @@
     </row>
     <row r="25" spans="9:23">
       <c r="I25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N25" s="4">
         <v>0.85</v>
@@ -4827,7 +4830,7 @@
     </row>
     <row r="31" spans="9:23" ht="15.75">
       <c r="I31" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
@@ -4839,7 +4842,7 @@
     </row>
     <row r="32" spans="9:23" ht="15.75">
       <c r="I32" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
@@ -4861,7 +4864,7 @@
     </row>
     <row r="34" spans="9:16" ht="15.75">
       <c r="I34" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
@@ -4897,7 +4900,7 @@
     </row>
     <row r="36" spans="9:16" ht="15.75">
       <c r="I36" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
@@ -4909,7 +4912,7 @@
     </row>
     <row r="37" spans="9:16" ht="15.75">
       <c r="I37" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
@@ -4921,7 +4924,7 @@
     </row>
     <row r="38" spans="9:16" ht="15.75">
       <c r="I38" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J38" s="17">
         <v>1363</v>
@@ -4947,7 +4950,7 @@
     </row>
     <row r="39" spans="9:16" ht="15.75">
       <c r="I39" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J39" s="17">
         <v>1363</v>
@@ -4973,7 +4976,7 @@
     </row>
     <row r="40" spans="9:16" ht="15.75">
       <c r="I40" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J40" s="17">
         <v>1363</v>
@@ -4999,7 +5002,7 @@
     </row>
     <row r="41" spans="9:16" ht="15.75">
       <c r="I41" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J41" s="18"/>
       <c r="K41" s="18"/>
@@ -5011,7 +5014,7 @@
     </row>
     <row r="42" spans="9:16" ht="15.75">
       <c r="I42" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J42" s="19">
         <v>34</v>
@@ -5037,7 +5040,7 @@
     </row>
     <row r="43" spans="9:16" ht="15.75">
       <c r="I43" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J43" s="19">
         <v>34</v>
@@ -5063,7 +5066,7 @@
     </row>
     <row r="44" spans="9:16" ht="15.75">
       <c r="I44" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J44" s="19">
         <v>34</v>
@@ -5089,7 +5092,7 @@
     </row>
     <row r="45" spans="9:16" ht="15.75">
       <c r="I45" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J45" s="18"/>
       <c r="K45" s="18"/>
@@ -5101,7 +5104,7 @@
     </row>
     <row r="46" spans="9:16" ht="15.75">
       <c r="I46" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J46" s="18"/>
       <c r="K46" s="18"/>
@@ -5113,7 +5116,7 @@
     </row>
     <row r="47" spans="9:16" ht="15.75">
       <c r="I47" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J47" s="17">
         <v>2470</v>
@@ -5139,7 +5142,7 @@
     </row>
     <row r="48" spans="9:16" ht="15.75">
       <c r="I48" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J48" s="17">
         <v>2470</v>
@@ -5165,7 +5168,7 @@
     </row>
     <row r="49" spans="9:16" ht="15.75">
       <c r="I49" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J49" s="17">
         <v>2470</v>
@@ -5191,7 +5194,7 @@
     </row>
     <row r="50" spans="9:16" ht="15.75">
       <c r="I50" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J50" s="18"/>
       <c r="K50" s="18"/>
@@ -5203,7 +5206,7 @@
     </row>
     <row r="51" spans="9:16" ht="15.75">
       <c r="I51" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J51" s="19">
         <v>62</v>
@@ -5229,7 +5232,7 @@
     </row>
     <row r="52" spans="9:16" ht="15.75">
       <c r="I52" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J52" s="19">
         <v>62</v>
@@ -5255,7 +5258,7 @@
     </row>
     <row r="53" spans="9:16" ht="15.75">
       <c r="I53" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J53" s="19">
         <v>62</v>
@@ -5291,7 +5294,7 @@
     </row>
     <row r="55" spans="9:16" ht="15.75">
       <c r="I55" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J55" s="12">
         <v>0.85</v>
@@ -5305,7 +5308,7 @@
     </row>
     <row r="56" spans="9:16" ht="15.75">
       <c r="I56" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
@@ -5317,7 +5320,7 @@
     </row>
     <row r="57" spans="9:16" ht="15.75">
       <c r="I57" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J57" s="12"/>
       <c r="K57" s="12"/>
@@ -5375,10 +5378,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12EA90E-43F0-4F26-A089-D51219939B11}">
-  <dimension ref="B3:X8"/>
+  <dimension ref="B3:Y8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5395,18 +5398,19 @@
     <col min="11" max="11" width="6.73046875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.796875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.9296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.46484375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.53125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="37.9296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.06640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.9296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.46484375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="37.9296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.06640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:24">
+    <row r="3" spans="2:25">
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -5414,7 +5418,7 @@
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
       <c r="H3" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
@@ -5424,18 +5428,19 @@
       <c r="N3" s="24"/>
       <c r="O3" s="24"/>
       <c r="P3" s="24"/>
-      <c r="Q3" s="24" t="s">
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="24"/>
       <c r="S3" s="24"/>
       <c r="T3" s="24"/>
       <c r="U3" s="24"/>
       <c r="V3" s="24"/>
       <c r="W3" s="24"/>
       <c r="X3" s="24"/>
-    </row>
-    <row r="4" spans="2:24">
+      <c r="Y3" s="24"/>
+    </row>
+    <row r="4" spans="2:25">
       <c r="B4" s="24" t="s">
         <v>1</v>
       </c>
@@ -5446,16 +5451,16 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" t="s">
         <v>91</v>
-      </c>
-      <c r="H4" t="s">
-        <v>92</v>
       </c>
       <c r="I4">
         <v>2030</v>
@@ -5464,98 +5469,105 @@
         <v>0</v>
       </c>
       <c r="K4" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="M4" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="O4" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="M4" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="N4" s="24" t="s">
+      <c r="P4" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="S4" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="U4" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="V4" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="W4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="X4" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="R4" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="S4" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="T4" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="U4" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="V4" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="W4" s="24" t="s">
+      <c r="Y4" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="X4" s="24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="2:24">
+    </row>
+    <row r="5" spans="2:25">
       <c r="B5" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" s="24">
         <v>0.90249999999999997</v>
       </c>
       <c r="L5" s="26">
+        <f>24/6</f>
         <v>4</v>
       </c>
       <c r="M5" s="24">
         <v>10</v>
       </c>
-      <c r="N5" s="26">
-        <v>3.6</v>
-      </c>
-      <c r="O5" s="24">
+      <c r="N5" s="24">
+        <v>150</v>
+      </c>
+      <c r="O5" s="26">
         <v>1</v>
       </c>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="R5" s="24" t="str">
+      <c r="P5" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="S5" s="24" t="str">
         <f>B5</f>
         <v>EV_Battery</v>
       </c>
-      <c r="S5" s="24" t="s">
-        <v>99</v>
-      </c>
       <c r="T5" s="24" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="U5" s="24" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="V5" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="W5" s="24"/>
+        <v>22</v>
+      </c>
+      <c r="W5" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="X5" s="24"/>
-    </row>
-    <row r="6" spans="2:24">
+      <c r="Y5" s="24"/>
+    </row>
+    <row r="6" spans="2:25">
       <c r="B6" s="24"/>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K6" s="24"/>
       <c r="L6" s="25">
@@ -5573,14 +5585,15 @@
       <c r="V6" s="24"/>
       <c r="W6" s="24"/>
       <c r="X6" s="24"/>
-    </row>
-    <row r="7" spans="2:24">
+      <c r="Y6" s="24"/>
+    </row>
+    <row r="7" spans="2:25">
       <c r="B7" s="24"/>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K7" s="24"/>
       <c r="L7" s="24"/>
@@ -5596,8 +5609,9 @@
       <c r="V7" s="24"/>
       <c r="W7" s="24"/>
       <c r="X7" s="24"/>
-    </row>
-    <row r="8" spans="2:24" ht="17.649999999999999">
+      <c r="Y7" s="24"/>
+    </row>
+    <row r="8" spans="2:25" ht="17.649999999999999">
       <c r="B8" s="21"/>
       <c r="E8" s="27"/>
       <c r="F8" t="str">
@@ -5609,7 +5623,7 @@
         <v>AuxStoIN</v>
       </c>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -5622,15 +5636,16 @@
       <c r="M8" s="22"/>
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
-      <c r="P8" s="21"/>
+      <c r="P8" s="22"/>
       <c r="Q8" s="21"/>
       <c r="R8" s="21"/>
       <c r="S8" s="21"/>
       <c r="T8" s="21"/>
       <c r="U8" s="21"/>
-      <c r="V8" s="23"/>
+      <c r="V8" s="21"/>
       <c r="W8" s="23"/>
       <c r="X8" s="23"/>
+      <c r="Y8" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-30 16:57
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_andHydro.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_andHydro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C43A57D-9155-42B6-8D3F-9A9646BBD5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66499C1-C7DF-4342-A94B-6EF4FBA1C6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2573" yWindow="2573" windowWidth="21600" windowHeight="12682" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="misc" sheetId="7" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-30 17:12
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_andHydro.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_andHydro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66499C1-C7DF-4342-A94B-6EF4FBA1C6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DE9EF7-E2FD-4D8B-BE69-3D6C5E31843F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2573" yWindow="2573" windowWidth="21600" windowHeight="12682" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3675" yWindow="3675" windowWidth="21600" windowHeight="12683" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="misc" sheetId="7" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-30 17:47
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_andHydro.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_REZoning_Sol_Win_andHydro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DE9EF7-E2FD-4D8B-BE69-3D6C5E31843F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB9BF49-BAD7-4C0D-A466-875BEE4F1E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="3675" windowWidth="21600" windowHeight="12683" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="misc" sheetId="7" r:id="rId1"/>

</xml_diff>